<commit_message>
Updated Sprint Backlog as per #28
End of day 3 updates to the backlog, also updated the Team Roster
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\Documents\3. Uni\Year 3\Agile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B68704-327A-424D-BE94-B17B1BAC6B56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C87C0E3-59E7-4425-8362-50CFEA480073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Story</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Display radius on map around the live location</t>
   </si>
   <si>
-    <t>Place a pin on the map at current location</t>
-  </si>
-  <si>
     <t>Choose radius to find locations in</t>
   </si>
   <si>
@@ -124,18 +121,6 @@
     <t>Retrieve information from pin</t>
   </si>
   <si>
-    <t>Stevn</t>
-  </si>
-  <si>
-    <t>Lchlano</t>
-  </si>
-  <si>
-    <t>cam</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Find design on boostrap</t>
   </si>
   <si>
@@ -158,13 +143,76 @@
   </si>
   <si>
     <t>Lachlan</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Nicole</t>
+  </si>
+  <si>
+    <t>Place a pin on the map at live location</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Cai</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Matriculation Number</t>
+  </si>
+  <si>
+    <t>Cameron McNeill</t>
+  </si>
+  <si>
+    <t>Steven Marshall</t>
+  </si>
+  <si>
+    <t>Lachlan Dow</t>
+  </si>
+  <si>
+    <t>Nicole Orr</t>
+  </si>
+  <si>
+    <t>Andrew Holligan</t>
+  </si>
+  <si>
+    <t>Cai Jingfan</t>
+  </si>
+  <si>
+    <t>2396229@dundee.ac.uk</t>
+  </si>
+  <si>
+    <t>ajholligan@dundee.ac.uk</t>
+  </si>
+  <si>
+    <t>nmorr@dundee.ac.uk</t>
+  </si>
+  <si>
+    <t>lxdow@dundee.ac.uk</t>
+  </si>
+  <si>
+    <t>stevenm682@gmail.com</t>
+  </si>
+  <si>
+    <t>cxmcneill@dundee.ac.uk</t>
+  </si>
+  <si>
+    <t>Email Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +220,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +239,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,10 +264,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -224,8 +293,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -351,24 +430,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Analytics!$A$5:$E$5</c:f>
+              <c:f>Analytics!$A$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,7 +484,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1285,16 +1364,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1587,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,11 +1686,11 @@
       <c r="B1" s="4"/>
       <c r="C1" s="3"/>
       <c r="D1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2"/>
       <c r="G1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
@@ -1634,22 +1713,22 @@
         <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1667,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1680,7 +1759,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1690,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1712,20 +1791,23 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5">
         <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M20" si="1">IF(D5 = 0,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -1733,6 +1815,9 @@
       <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
@@ -1745,27 +1830,42 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8">
         <v>1</v>
       </c>
       <c r="M8" t="str">
@@ -1786,7 +1886,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
@@ -1796,7 +1896,7 @@
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1805,6 +1905,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
@@ -1812,20 +1915,23 @@
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -1835,14 +1941,20 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
@@ -1852,7 +1964,7 @@
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -1861,6 +1973,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
       <c r="M13" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
@@ -1869,14 +1984,20 @@
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="1"/>
@@ -1885,10 +2006,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1898,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H15">
         <v>2</v>
@@ -1910,34 +2031,46 @@
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16">
         <v>5</v>
       </c>
       <c r="M16" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
       <c r="M17" s="6" t="str">
         <f t="shared" si="1"/>
@@ -1947,7 +2080,7 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -1956,6 +2089,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
       <c r="M18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
@@ -1964,7 +2100,7 @@
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1973,6 +2109,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
       <c r="M19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
@@ -1981,7 +2120,7 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -1989,6 +2128,9 @@
       <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
       </c>
       <c r="M20" s="6" t="str">
         <f t="shared" si="1"/>
@@ -2019,80 +2161,190 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="13">
+        <v>170014393</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="13">
+        <v>170008935</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="13">
+        <v>170010225</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="13">
+        <v>170010591</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="13">
+        <v>170014201</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="13">
+        <v>2396229</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{844BCE0C-0B45-4CBA-A917-C91F25304E54}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{3F4DE484-F450-4899-B991-51211C814E3E}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{81B93ED2-BA34-4C68-BD1B-BF36669B8EF6}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{70D9AEFE-795C-451E-8DA5-2365D06D8266}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{9D5492E9-B67B-4B10-8698-8049CBB6D05A}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{615CB111-0127-49C3-8763-C55D03D892BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SUM('Sprint 2 Backlog'!C:C)</f>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:G)</f>
-        <v>44</v>
-      </c>
-      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="B6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:H)</f>
-        <v>40</v>
-      </c>
-      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="C6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:I)</f>
-        <v>40</v>
-      </c>
-      <c r="D5">
+        <v>22</v>
+      </c>
+      <c r="D6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:J)</f>
-        <v>40</v>
-      </c>
-      <c r="E5">
+        <v>22</v>
+      </c>
+      <c r="E6">
         <f>$A$2 - SUM('Sprint 2 Backlog'!G:K)</f>
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>